<commit_message>
made a resetSignal request
</commit_message>
<xml_diff>
--- a/attendance.xlsx
+++ b/attendance.xlsx
@@ -8,6 +8,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="2020-11-02" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="2020-11-08" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -475,4 +476,111 @@
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Sr. No</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Name</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Address</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Job</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Time-Stamp</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>SpO2_value</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>14:24:41</t>
+        </is>
+      </c>
+      <c r="F2" t="n">
+        <v>93.10171335021791</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>sachin</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>xyz/xyz</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>coder</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>14:26:27</t>
+        </is>
+      </c>
+      <c r="F3" t="n">
+        <v>93.83166958817134</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
 </file>
</xml_diff>